<commit_message>
Problem 1-9 and 11 solved
</commit_message>
<xml_diff>
--- a/EasyAssetManager/wwwroot/UserSpace/SUMAN.BANERJEE/LOAN_RM_TARGET.xlsx
+++ b/EasyAssetManager/wwwroot/UserSpace/SUMAN.BANERJEE/LOAN_RM_TARGET.xlsx
@@ -541,8 +541,8 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,35 +562,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>6</v>
@@ -607,28 +607,28 @@
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="6">
+      <c r="E2" s="6">
         <v>124</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
       <c r="K2" s="1">
         <v>100</v>
       </c>
@@ -639,31 +639,31 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
       <c r="K3" s="1">
         <v>50</v>
       </c>
@@ -674,31 +674,31 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
       <c r="K4" s="1">
         <v>200</v>
       </c>

</xml_diff>